<commit_message>
adding latest public version
</commit_message>
<xml_diff>
--- a/dna_workflow_db.xlsx
+++ b/dna_workflow_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cunningr/git-projects/EMEAR-Enterprise-Networking/python/dna_workflows/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cunningr/git-projects/dna_workflows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0536B8E7-E256-3946-B646-69088CA3E71B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E43C53D-30F7-FC4A-9A54-28BC7938E4E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,8 @@
     <sheet name="workflows" sheetId="1" r:id="rId1"/>
     <sheet name="sites" sheetId="2" r:id="rId2"/>
     <sheet name="ip_pool" sheetId="3" r:id="rId3"/>
-    <sheet name="discovery" sheetId="5" r:id="rId4"/>
-    <sheet name="border_handoff" sheetId="6" r:id="rId5"/>
-    <sheet name="control" sheetId="7" r:id="rId6"/>
+    <sheet name="discovery" sheetId="4" r:id="rId4"/>
+    <sheet name="control" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="statu" localSheetId="2">presence[presence]</definedName>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="134">
   <si>
     <t>api_version</t>
   </si>
@@ -49,15 +48,6 @@
     <t>1.3.0</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>C!sc0123</t>
-  </si>
-  <si>
-    <t>https://127.0.0.1:8888</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -70,39 +60,39 @@
     <t>Description</t>
   </si>
   <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>sites</t>
+  </si>
+  <si>
+    <t>Create, Delete of DNA Center site hierarchy</t>
+  </si>
+  <si>
+    <t>ip_pool</t>
+  </si>
+  <si>
+    <t>Create, Delete of DNA Center IP Pools</t>
+  </si>
+  <si>
+    <t>discovery</t>
+  </si>
+  <si>
+    <t>Update this workflow documentation</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
     <t>enabled</t>
   </si>
   <si>
-    <t>sites</t>
-  </si>
-  <si>
-    <t>Create, Delete of DNA Center site hierarchy</t>
-  </si>
-  <si>
-    <t>ip_pool</t>
-  </si>
-  <si>
-    <t>Create, Delete of DNA Center IP Pools</t>
-  </si>
-  <si>
-    <t>discovery</t>
-  </si>
-  <si>
-    <t>Update this workflow documentation</t>
-  </si>
-  <si>
-    <t>border_handoff</t>
-  </si>
-  <si>
-    <t>Stage</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
     <t>create</t>
   </si>
   <si>
@@ -118,363 +108,309 @@
     <t>presence</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>parentName</t>
+  </si>
+  <si>
+    <t>absent</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Global/UK</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>Global/US</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>APAC</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Cisco Reading</t>
+  </si>
+  <si>
+    <t>Global/UK/Reading</t>
+  </si>
+  <si>
+    <t>300 Longwater Avenue</t>
+  </si>
+  <si>
+    <t>Cisco SJ</t>
+  </si>
+  <si>
+    <t>Global/US/SJ</t>
+  </si>
+  <si>
+    <t>260 E Tasman Dr</t>
+  </si>
+  <si>
+    <t>San Jose</t>
+  </si>
+  <si>
+    <t>rfModel</t>
+  </si>
+  <si>
+    <t>floor 1</t>
+  </si>
+  <si>
+    <t>Global/UK/Reading/Cisco Reading</t>
+  </si>
+  <si>
+    <t>Indoor High Ceiling</t>
+  </si>
+  <si>
+    <t>Global/US/SJ/Cisco SJ</t>
+  </si>
+  <si>
+    <t>Cubes And Walled Offices</t>
+  </si>
+  <si>
+    <t>floor 2</t>
+  </si>
+  <si>
+    <t>create_pools</t>
+  </si>
+  <si>
+    <t>Creates IP pools</t>
+  </si>
+  <si>
+    <t>create_reservations</t>
+  </si>
+  <si>
+    <t>Creates IP reservations</t>
+  </si>
+  <si>
+    <t>delete_pools</t>
+  </si>
+  <si>
+    <t>Deletes IP pools</t>
+  </si>
+  <si>
+    <t>delete_reservations</t>
+  </si>
+  <si>
+    <t>Deletes IP reservations</t>
+  </si>
+  <si>
+    <t>ipPoolName</t>
+  </si>
+  <si>
+    <t>ipPoolCidr</t>
+  </si>
+  <si>
+    <t>gateways</t>
+  </si>
+  <si>
+    <t>dhcpServerIps</t>
+  </si>
+  <si>
+    <t>dnsServerIps</t>
+  </si>
+  <si>
+    <t>cunningr_1</t>
+  </si>
+  <si>
+    <t>90.0.0.0/24</t>
+  </si>
+  <si>
+    <t>cunningr_2</t>
+  </si>
+  <si>
+    <t>90.0.1.0/24</t>
+  </si>
+  <si>
+    <t>cunningr_4</t>
+  </si>
+  <si>
+    <t>90.0.2.0./24</t>
+  </si>
+  <si>
+    <t>cunningr_5</t>
+  </si>
+  <si>
+    <t>90.0.3.0/24</t>
+  </si>
+  <si>
+    <t>groupName</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
-    <t>site.area.name</t>
-  </si>
-  <si>
-    <t>site.area.parentName</t>
+    <t>ipReservation</t>
+  </si>
+  <si>
+    <t>siteName</t>
+  </si>
+  <si>
+    <t>ipPoolsParent</t>
+  </si>
+  <si>
+    <t>cunningr_1_res</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>1.1.1.1,1.1.1.2</t>
+  </si>
+  <si>
+    <t>90.0.0.1</t>
+  </si>
+  <si>
+    <t>cunningr_2_res</t>
+  </si>
+  <si>
+    <t>cunningr_4_res</t>
+  </si>
+  <si>
+    <t>cunningr_5_res</t>
+  </si>
+  <si>
+    <t>create_global_credentials</t>
+  </si>
+  <si>
+    <t>Creates global credintials for CLI/SNMPv2c</t>
+  </si>
+  <si>
+    <t>delete_global_credentials</t>
+  </si>
+  <si>
+    <t>Deletes global credintials for CLI/SNMPv2c</t>
+  </si>
+  <si>
+    <t>run_discovery</t>
+  </si>
+  <si>
+    <t>Creates and runs new discovery jobs</t>
+  </si>
+  <si>
+    <t>delete_discovery</t>
+  </si>
+  <si>
+    <t>Deletes discovery jobs</t>
+  </si>
+  <si>
+    <t>credentialType</t>
+  </si>
+  <si>
+    <t>writeCommunity</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>GLOBAL</t>
+  </si>
+  <si>
+    <t>it54s3cret</t>
+  </si>
+  <si>
+    <t>what is this?</t>
+  </si>
+  <si>
+    <t>snmp_rw_dna_workflows</t>
+  </si>
+  <si>
+    <t>readCommunity</t>
+  </si>
+  <si>
+    <t>snmp_ro_dna_workflows</t>
+  </si>
+  <si>
+    <t>enablePassword</t>
+  </si>
+  <si>
+    <t>dna_workflows</t>
+  </si>
+  <si>
+    <t>cli_creds_dna_workflows</t>
+  </si>
+  <si>
+    <t>discoveryType</t>
+  </si>
+  <si>
+    <t>preferredMgmtIPMethod</t>
+  </si>
+  <si>
+    <t>startIp</t>
+  </si>
+  <si>
+    <t>endIp</t>
+  </si>
+  <si>
+    <t>cli</t>
+  </si>
+  <si>
+    <t>snmp_ro</t>
+  </si>
+  <si>
+    <t>snmp_rw</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>UseLoopBack</t>
+  </si>
+  <si>
+    <t>10.0.0.0</t>
+  </si>
+  <si>
+    <t>10.0.0.255</t>
+  </si>
+  <si>
+    <t>discovery_dna_workflows</t>
   </si>
   <si>
     <t>present</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>siteType</t>
+  </si>
+  <si>
     <t>area</t>
   </si>
   <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>Reading</t>
-  </si>
-  <si>
-    <t>Global/UK</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>SJ</t>
-  </si>
-  <si>
-    <t>Global/US</t>
-  </si>
-  <si>
-    <t>EU</t>
-  </si>
-  <si>
-    <t>APAC</t>
-  </si>
-  <si>
-    <t>site.building.name</t>
-  </si>
-  <si>
-    <t>site.building.address</t>
-  </si>
-  <si>
-    <t>site.building.parentName</t>
-  </si>
-  <si>
-    <t>site.building.latitude</t>
-  </si>
-  <si>
-    <t>site.building.longitude</t>
-  </si>
-  <si>
     <t>building</t>
   </si>
   <si>
-    <t>Cisco Reading</t>
-  </si>
-  <si>
-    <t>300 Longwater Avenue</t>
-  </si>
-  <si>
-    <t>Global/UK/Reading</t>
-  </si>
-  <si>
-    <t>Cisco SJ</t>
-  </si>
-  <si>
-    <t>1 Cisco Way</t>
-  </si>
-  <si>
-    <t>Global/US/SJ</t>
-  </si>
-  <si>
-    <t>site.floor.name</t>
-  </si>
-  <si>
-    <t>site.floor.parentName</t>
-  </si>
-  <si>
-    <t>site.floor.width</t>
-  </si>
-  <si>
-    <t>site.floor.length</t>
-  </si>
-  <si>
-    <t>site.floor.height</t>
-  </si>
-  <si>
-    <t>site.floor.rfModel</t>
-  </si>
-  <si>
     <t>floor</t>
   </si>
   <si>
-    <t>floor 1</t>
-  </si>
-  <si>
-    <t>Global/UK/Reading/Cisco Reading</t>
-  </si>
-  <si>
-    <t>Indoor High Ceiling</t>
-  </si>
-  <si>
-    <t>Global/US/SJ/Cisco SJ</t>
-  </si>
-  <si>
-    <t>Cubes And Walled Offices</t>
-  </si>
-  <si>
-    <t>floor 2</t>
-  </si>
-  <si>
-    <t>create_pools</t>
-  </si>
-  <si>
-    <t>Creates IP pools</t>
-  </si>
-  <si>
-    <t>create_reservations</t>
-  </si>
-  <si>
-    <t>Creates IP reservations</t>
-  </si>
-  <si>
-    <t>delete_pools</t>
-  </si>
-  <si>
-    <t>Deletes IP pools</t>
-  </si>
-  <si>
-    <t>delete_reservations</t>
-  </si>
-  <si>
-    <t>Deletes IP reservations</t>
-  </si>
-  <si>
-    <t>ipPoolName</t>
-  </si>
-  <si>
-    <t>ipPoolCidr</t>
-  </si>
-  <si>
-    <t>gateways</t>
-  </si>
-  <si>
-    <t>dhcpServerIps</t>
-  </si>
-  <si>
-    <t>dnsServerIps</t>
-  </si>
-  <si>
-    <t>absent</t>
-  </si>
-  <si>
-    <t>cunningr_1</t>
-  </si>
-  <si>
-    <t>90.0.0.0/24</t>
-  </si>
-  <si>
-    <t>cunningr_2</t>
-  </si>
-  <si>
-    <t>90.0.1.0/24</t>
-  </si>
-  <si>
-    <t>cunningr_4</t>
-  </si>
-  <si>
-    <t>90.0.2.0./24</t>
-  </si>
-  <si>
-    <t>cunningr_5</t>
-  </si>
-  <si>
-    <t>90.0.3.0/24</t>
-  </si>
-  <si>
-    <t>groupName</t>
-  </si>
-  <si>
-    <t>ipPools.ipPoolCidr</t>
-  </si>
-  <si>
-    <t>siteName</t>
-  </si>
-  <si>
-    <t>ipPools.parent</t>
-  </si>
-  <si>
-    <t>ipPools.dhcpServerIps</t>
-  </si>
-  <si>
-    <t>ipPools.dnsServerIps</t>
-  </si>
-  <si>
-    <t>ipPools.gateways</t>
-  </si>
-  <si>
-    <t>cunningr_1_res</t>
-  </si>
-  <si>
-    <t>generic</t>
-  </si>
-  <si>
-    <t>1.1.1.1,1.1.1.2</t>
-  </si>
-  <si>
-    <t>90.0.0.1</t>
-  </si>
-  <si>
-    <t>cunningr_2_res</t>
-  </si>
-  <si>
-    <t>cunningr_4_res</t>
-  </si>
-  <si>
-    <t>cunningr_5_res</t>
-  </si>
-  <si>
-    <t>create_global_credentials</t>
-  </si>
-  <si>
-    <t>Creates global credintials for CLI/SNMPv2c</t>
-  </si>
-  <si>
-    <t>delete_global_credentials</t>
-  </si>
-  <si>
-    <t>Deletes global credintials for CLI/SNMPv2c</t>
-  </si>
-  <si>
-    <t>run_discovery</t>
-  </si>
-  <si>
-    <t>Creates and runs new discovery jobs</t>
-  </si>
-  <si>
-    <t>delete_discovery</t>
-  </si>
-  <si>
-    <t>Deletes discovery jobs</t>
-  </si>
-  <si>
-    <t>credentialType</t>
-  </si>
-  <si>
-    <t>writeCommunity</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>GLOBAL</t>
-  </si>
-  <si>
-    <t>it54s3cret</t>
-  </si>
-  <si>
-    <t>what is this?</t>
-  </si>
-  <si>
-    <t>snmp_rw_dna_workflows</t>
-  </si>
-  <si>
-    <t>readCommunity</t>
-  </si>
-  <si>
-    <t>snmp_ro_dna_workflows</t>
-  </si>
-  <si>
-    <t>enablePassword</t>
-  </si>
-  <si>
-    <t>dna_workflows</t>
-  </si>
-  <si>
-    <t>cli_creds_dna_workflows</t>
-  </si>
-  <si>
-    <t>discoveryType</t>
-  </si>
-  <si>
-    <t>preferredMgmtIPMethod</t>
-  </si>
-  <si>
-    <t>startIp</t>
-  </si>
-  <si>
-    <t>endIp</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>cli</t>
-  </si>
-  <si>
-    <t>snmp_ro</t>
-  </si>
-  <si>
-    <t>snmp_rw</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>UseLoopBack</t>
-  </si>
-  <si>
-    <t>10.0.0.0</t>
-  </si>
-  <si>
-    <t>10.0.0.255</t>
-  </si>
-  <si>
-    <t>discovery_dna_workflows</t>
-  </si>
-  <si>
-    <t>get_borders</t>
-  </si>
-  <si>
-    <t>Gets configuration of border devices from table</t>
-  </si>
-  <si>
-    <t>border_ip</t>
-  </si>
-  <si>
-    <t>hostname</t>
-  </si>
-  <si>
-    <t>192.168.0.3</t>
-  </si>
-  <si>
-    <t>border1.lab.cisco.com</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>disabled</t>
-  </si>
-  <si>
-    <t>siteType</t>
-  </si>
-  <si>
-    <t>rfModel</t>
-  </si>
-  <si>
     <t>Drywall Office Only</t>
   </si>
   <si>
@@ -485,6 +421,15 @@
   </si>
   <si>
     <t>1.2.10</t>
+  </si>
+  <si>
+    <t>devnetuser</t>
+  </si>
+  <si>
+    <t>Cisco123!</t>
+  </si>
+  <si>
+    <t>https://sandboxdnac2.cisco.com:443</t>
   </si>
 </sst>
 </file>
@@ -603,11 +548,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -619,12 +563,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="38">
     <dxf>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
@@ -1106,138 +1052,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left/>
         <right/>
@@ -1565,8 +1379,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="workflow" displayName="workflow" ref="B6:E10" totalsRowShown="0">
-  <autoFilter ref="B6:E10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="workflow" displayName="workflow" ref="B6:E9" totalsRowShown="0">
+  <autoFilter ref="B6:E9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Status"/>
@@ -1578,128 +1392,124 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="control?discovery?Function" displayName="control?discovery?Function" ref="B2:E6">
-  <autoFilter ref="B2:E6" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="control?discovery?Function" displayName="control?discovery?Function" ref="B2:E6">
+  <autoFilter ref="B2:E6" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Stage"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Status"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Function"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Documentation"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Stage"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Status"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Task"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Documentation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="native?snmpWrite?description" displayName="native?snmpWrite?description" ref="B9:F10" totalsRowShown="0">
-  <autoFilter ref="B9:F10" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="native?snmpWrite?description" displayName="native?snmpWrite?description" ref="B9:F10" totalsRowShown="0">
+  <autoFilter ref="B9:F10" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="presence"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="credentialType"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="writeCommunity"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="comments"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="native?snmpRead?description" displayName="native?snmpRead?description" ref="B12:F13" totalsRowShown="0">
+  <autoFilter ref="B12:F13" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="presence"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="credentialType"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="readCommunity"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="comments"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="native?cli?description" displayName="native?cli?description" ref="B15:G16" totalsRowShown="0">
+  <autoFilter ref="B15:G16" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+  <tableColumns count="6">
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="presence"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="credentialType"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="writeCommunity"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="comments"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="username"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="password"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="enablePassword"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="native?snmpRead?description" displayName="native?snmpRead?description" ref="B12:F13" totalsRowShown="0">
-  <autoFilter ref="B12:F13" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="presence"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="credentialType"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="readCommunity"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="comments"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="description"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="native?cli?description" displayName="native?cli?description" ref="B15:G16" totalsRowShown="0">
-  <autoFilter ref="B15:G16" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="presence"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="credentialType"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="username"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="password"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="enablePassword"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="description"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="native?discovery?name" displayName="native?discovery?name" ref="B18:J19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="B18:J19" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="native?discovery?name" displayName="native?discovery?name" ref="B18:J19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="B18:J19" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="presence" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="discoveryType" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="preferredMgmtIPMethod" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="startIp" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="endIp" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="name" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0F00-000007000000}" name="cli" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0F00-000008000000}" name="snmp_ro" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0F00-000009000000}" name="snmp_rw" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="presence" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="discoveryType" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="preferredMgmtIPMethod" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="startIp" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="endIp" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="name" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="cli" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="snmp_ro" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="snmp_rw" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="control?border_handoff?Function" displayName="control?border_handoff?Function" ref="B2:E3">
-  <autoFilter ref="B2:E3" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Stage"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Status"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Function"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Documentation"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="presence" displayName="presence" ref="B2:B4" totalsRowShown="0">
+  <autoFilter ref="B2:B4" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="presence"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="native?border_handoff?border_ip" displayName="native?border_handoff?border_ip" ref="B7:C8" totalsRowShown="0">
-  <autoFilter ref="B7:C8" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="border_ip"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="hostname"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="status" displayName="status" ref="B6:B8" totalsRowShown="0">
+  <autoFilter ref="B6:B8" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="presence" displayName="presence" ref="B2:B4" totalsRowShown="0">
-  <autoFilter ref="B2:B4" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="siteType" displayName="siteType" ref="B10:B13" totalsRowShown="0">
+  <autoFilter ref="B10:B13" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="presence"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="siteType"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="status" displayName="status" ref="B6:B8" totalsRowShown="0">
-  <autoFilter ref="B6:B8" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="floors.rfModel" displayName="floors.rfModel" ref="B15:B20" totalsRowShown="0">
+  <autoFilter ref="B15:B20" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="rfModel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="siteType" displayName="siteType" ref="B10:B13" totalsRowShown="0">
-  <autoFilter ref="B10:B13" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="boolean" displayName="boolean" ref="B22:B24" totalsRowShown="0">
+  <autoFilter ref="B22:B24" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="siteType"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="boolean"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1720,76 +1530,50 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="floors.rfModel" displayName="floors.rfModel" ref="B15:B20" totalsRowShown="0">
-  <autoFilter ref="B15:B20" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="api_versions" displayName="api_versions" ref="B26:B28" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="B26:B28" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="rfModel"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="boolean" displayName="boolean" ref="B22:B24" totalsRowShown="0">
-  <autoFilter ref="B22:B24" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="boolean"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="api_versions" displayName="api_versions" ref="B26:B28" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="B26:B28" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="api_version" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="api_version" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="native?sites?site.area.name" displayName="native?sites?site.area.name" ref="B6:E13" totalsRowShown="0">
-  <autoFilter ref="B6:E13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="native?sites?areas" displayName="native?sites?areas" ref="B6:D12" totalsRowShown="0">
+  <autoFilter ref="B6:D12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="3">
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="presence"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="type"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="site.area.name"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="site.area.parentName"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="name"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="parentName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="native?buildings?site.building.name" displayName="native?buildings?site.building.name" ref="B15:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
-  <autoFilter ref="B15:H17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="presence" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="type" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="site.building.name" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="site.building.address"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="site.building.parentName" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="site.building.latitude" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="site.building.longitude" dataDxfId="31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="native?sites?buildings" displayName="native?sites?buildings" ref="B14:G16" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B14:G16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="presence" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="name" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="parentName" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="street" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="city" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="country" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="native?floors?site.floor.parentName" displayName="native?floors?site.floor.parentName" ref="B19:I22" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B19:I22" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="presence" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="site.floor.name" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="site.floor.parentName" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="site.floor.width" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="site.floor.length" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="site.floor.height" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="site.floor.rfModel" dataDxfId="18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="native?sites?floors" displayName="native?sites?floors" ref="B18:E21" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="B18:E21" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="presence" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="name" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="parentName" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="rfModel" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1801,7 +1585,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Stage"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Status"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Function"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Task"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Documentation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1809,7 +1593,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="native?ip_pools?ipPoolName" displayName="native?ip_pools?ipPoolName" ref="B8:G12" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="native?ip_pool?ip_pools" displayName="native?ip_pool?ip_pools" ref="B8:G12" totalsRowShown="0">
   <autoFilter ref="B8:G12" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="6">
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="presence"/>
@@ -1824,18 +1608,18 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="native?ip_groups?groupName" displayName="native?ip_groups?groupName" ref="B14:J18" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="native?ip_pool?ip_reservations" displayName="native?ip_pool?ip_reservations" ref="B14:J18" totalsRowShown="0">
   <autoFilter ref="B14:J18" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="9">
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="presence"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="groupName"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="type"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="ipPools.ipPoolCidr"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="ipReservation"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="siteName"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="ipPools.parent"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="ipPools.dhcpServerIps"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="ipPools.dnsServerIps"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="ipPools.gateways"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="ipPoolsParent"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="dhcpServerIps"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="dnsServerIps"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="gateways"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1847,7 +1631,7 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Stage"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Status"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Function"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Task"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Documentation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2154,10 +1938,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B3:F10"/>
+  <dimension ref="B3:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2190,13 +1974,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>132</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -2204,16 +1988,16 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -2221,13 +2005,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -2235,13 +2019,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
@@ -2249,45 +2033,31 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT("boolean[boolean]")</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>INDIRECT("api_versions[api_version]")</formula1>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C7:C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
+      <formula1>INDIRECT("status[status]")</formula1>
+    </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2297,10 +2067,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B19" sqref="B19:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2309,7 +2079,7 @@
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.1640625" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.83203125" bestFit="1" customWidth="1"/>
@@ -2317,341 +2087,249 @@
     <col min="11" max="11" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>36</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="E19" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="3">
-        <v>50</v>
-      </c>
-      <c r="H16" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="1" t="s">
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E20" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="1" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="3">
-        <v>60</v>
-      </c>
-      <c r="H17" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20">
-        <v>50</v>
-      </c>
-      <c r="G20">
-        <v>50</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21">
-        <v>50</v>
-      </c>
-      <c r="G21">
-        <v>50</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22">
-        <v>50</v>
-      </c>
-      <c r="G22">
-        <v>50</v>
-      </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
-        <v>66</v>
+      <c r="D21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B16:B17 B7:B13 B20:B22" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B15:B16 B7:B12 B19:B21" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>INDIRECT("presence[presence]")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I20" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E19" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>INDIRECT("floors.rfModel[rfModel]")</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C4" xr:uid="{00000000-0002-0000-0100-000002000000}">
@@ -2676,7 +2354,7 @@
   <dimension ref="B2:J18"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E3"/>
+      <selection activeCell="B15" sqref="B15:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2695,16 +2373,16 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -2712,13 +2390,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -2726,13 +2404,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
@@ -2740,13 +2418,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
@@ -2754,192 +2432,192 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="J14" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>81</v>
       </c>
-      <c r="C15" t="s">
-        <v>97</v>
-      </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
         <v>83</v>
       </c>
-      <c r="F15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15" t="s">
-        <v>99</v>
-      </c>
       <c r="J15" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2964,14 +2642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2988,16 +2666,16 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
@@ -3005,13 +2683,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
@@ -3019,13 +2697,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
@@ -3033,13 +2711,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
@@ -3047,89 +2725,89 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -3138,105 +2816,105 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G15" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>119</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 B13 B16 B19" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 B16 B13 B19" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>INDIRECT("presence[presence]")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C6" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C3:C6" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>INDIRECT("status[status]")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I19" xr:uid="{00000000-0002-0000-0400-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I19" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>INDIRECT("native?snmpRead?description[description]")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H19" xr:uid="{00000000-0002-0000-0400-000003000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H19" xr:uid="{00000000-0002-0000-0300-000003000000}">
       <formula1>INDIRECT("native?cli?description[description]")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J19" xr:uid="{00000000-0002-0000-0400-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J19" xr:uid="{00000000-0002-0000-0300-000004000000}">
       <formula1>INDIRECT("native?snmpWrite?description[description]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -3252,79 +2930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="B2:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
@@ -3342,82 +2948,82 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>145</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
@@ -3436,12 +3042,12 @@
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
-        <v>151</v>
+      <c r="B27" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>